<commit_message>
updated mapping file with sex ratio and esacpement jack numbers
</commit_message>
<xml_diff>
--- a/termNIT/2023/TERMNIT_mapping_2023.xlsx
+++ b/termNIT/2023/TERMNIT_mapping_2023.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\WCVI_Chinook_Term_Run_Recon\WCVI_CN_TermRunRecon\termNIT\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD2CD2A-33C0-4B27-A69A-B17432BEAAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1582F3A0-BD9D-487A-BDF8-B7793FDD4BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{E2731BFC-E1F4-4F7A-AD91-46B95AB44FF5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="1" xr2:uid="{E2731BFC-E1F4-4F7A-AD91-46B95AB44FF5}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
     <sheet name="termNIT_map" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">termNIT_map!$C$2:$R$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">termNIT_map!$C$2:$R$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -230,7 +230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="93">
   <si>
     <t>FSC</t>
   </si>
@@ -498,12 +498,24 @@
   <si>
     <t>TermRun_AGEStemp</t>
   </si>
+  <si>
+    <t>Escapement - sex/age correction</t>
+  </si>
+  <si>
+    <t>Actual sex ratio (from hatchery staff)</t>
+  </si>
+  <si>
+    <t>Adults</t>
+  </si>
+  <si>
+    <t>Total (incl Jacks)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,6 +552,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -570,10 +589,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -593,9 +613,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -50146,17 +50170,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD15511-D0E0-440B-B215-63E04B9AC67B}">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -51457,7 +51481,7 @@
         <v>51</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>14</v>
@@ -51501,7 +51525,7 @@
         <v>80</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>10</v>
@@ -51510,13 +51534,13 @@
         <v>51</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J27" s="4">
-        <v>0</v>
+        <v>14250</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>73</v>
@@ -51566,7 +51590,7 @@
         <v>15</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="J28" s="4">
         <v>0</v>
@@ -51619,7 +51643,7 @@
         <v>15</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J29" s="4">
         <v>0</v>
@@ -51672,7 +51696,7 @@
         <v>15</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J30" s="4">
         <v>0</v>
@@ -51725,7 +51749,7 @@
         <v>15</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J31" s="4">
         <v>0</v>
@@ -51756,6 +51780,209 @@
       </c>
       <c r="S31" s="4">
         <v>2022</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J32" s="4">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P32" s="4">
+        <v>2023</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="S32" s="4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" s="7">
+        <v>0.54877848827676701</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P33" s="4">
+        <v>2023</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S33" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="7">
+        <v>0.43613707165109</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P34" s="4">
+        <v>2023</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S34" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J35" s="7">
+        <v>1.5084440072142999E-2</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P35" s="4">
+        <v>2023</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R35" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to mapping file
</commit_message>
<xml_diff>
--- a/termNIT/2023/TERMNIT_mapping_2023.xlsx
+++ b/termNIT/2023/TERMNIT_mapping_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\WCVI_Chinook_Term_Run_Recon\WCVI_CN_TermRunRecon\termNIT\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1582F3A0-BD9D-487A-BDF8-B7793FDD4BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832F2970-95A8-45A5-AEBC-78F4EDB8DA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="1" xr2:uid="{E2731BFC-E1F4-4F7A-AD91-46B95AB44FF5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{E2731BFC-E1F4-4F7A-AD91-46B95AB44FF5}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -230,7 +230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="94">
   <si>
     <t>FSC</t>
   </si>
@@ -421,15 +421,6 @@
     <t>Broostock corrected - Total</t>
   </si>
   <si>
-    <t>Broostock corrected - Males</t>
-  </si>
-  <si>
-    <t>Broodstock corrected - Females</t>
-  </si>
-  <si>
-    <t>Broodstock corrected - Jacks</t>
-  </si>
-  <si>
     <t>Broodstock corrected - Total</t>
   </si>
   <si>
@@ -455,15 +446,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Broodstock, morts, other - Males</t>
-  </si>
-  <si>
-    <t>Broodstock, morts, other - Females</t>
-  </si>
-  <si>
-    <t>Broodstock, morts, other - Jacks</t>
   </si>
   <si>
     <t>Broodstock, morts, other - Total</t>
@@ -509,6 +491,27 @@
   </si>
   <si>
     <t>Total (incl Jacks)</t>
+  </si>
+  <si>
+    <t>Broodstock, morts, other - Males (incl Jacks)</t>
+  </si>
+  <si>
+    <t>Broodstock, morts, other - Male</t>
+  </si>
+  <si>
+    <t>Broodstock, morts, other - Female</t>
+  </si>
+  <si>
+    <t>Broodstock, morts, other - Jack</t>
+  </si>
+  <si>
+    <t>Broodstock corrected - Jack</t>
+  </si>
+  <si>
+    <t>Broodstock corrected - Female</t>
+  </si>
+  <si>
+    <t>Broodstock corrected</t>
   </si>
 </sst>
 </file>
@@ -613,7 +616,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -50172,7 +50175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD15511-D0E0-440B-B215-63E04B9AC67B}">
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
@@ -50192,7 +50195,8 @@
     <col min="12" max="12" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="34.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="35.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="35.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="50.85546875" style="4" customWidth="1"/>
+    <col min="16" max="16" width="35.7109375" style="4" customWidth="1"/>
     <col min="17" max="17" width="34.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="35.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21.85546875" style="4" bestFit="1" customWidth="1"/>
@@ -50201,21 +50205,21 @@
   <sheetData>
     <row r="1" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>36</v>
@@ -50242,31 +50246,31 @@
         <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="S2" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
@@ -50274,7 +50278,7 @@
         <v>2023</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>35</v>
@@ -50292,10 +50296,10 @@
         <v>22</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>24</v>
@@ -50324,7 +50328,7 @@
         <v>2023</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>35</v>
@@ -50342,10 +50346,10 @@
         <v>22</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>24</v>
@@ -50374,7 +50378,7 @@
         <v>2023</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>35</v>
@@ -50395,10 +50399,10 @@
         <v>900</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>24</v>
@@ -50427,7 +50431,7 @@
         <v>2023</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>35</v>
@@ -50448,10 +50452,10 @@
         <v>4768</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>24</v>
@@ -50480,7 +50484,7 @@
         <v>2023</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>35</v>
@@ -50501,10 +50505,10 @@
         <v>3233</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>24</v>
@@ -50533,7 +50537,7 @@
         <v>2023</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>35</v>
@@ -50554,10 +50558,10 @@
         <v>8001</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>24</v>
@@ -50586,7 +50590,7 @@
         <v>2023</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>2</v>
@@ -50607,10 +50611,10 @@
         <v>277</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>31</v>
@@ -50639,7 +50643,7 @@
         <v>2023</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>2</v>
@@ -50660,10 +50664,10 @@
         <v>6</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>31</v>
@@ -50692,7 +50696,7 @@
         <v>2023</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>2</v>
@@ -50745,7 +50749,7 @@
         <v>2023</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>2</v>
@@ -50795,7 +50799,7 @@
         <v>2023</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>2</v>
@@ -50845,7 +50849,7 @@
         <v>2023</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>2</v>
@@ -50863,10 +50867,10 @@
         <v>0</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>24</v>
@@ -50895,7 +50899,7 @@
         <v>2023</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>2</v>
@@ -50913,10 +50917,10 @@
         <v>300</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>24</v>
@@ -50945,7 +50949,7 @@
         <v>2023</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>6</v>
@@ -50995,7 +50999,7 @@
         <v>2023</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>6</v>
@@ -51045,7 +51049,7 @@
         <v>2023</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>11</v>
@@ -51066,10 +51070,10 @@
         <v>2747</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>32</v>
@@ -51078,7 +51082,7 @@
         <v>32</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="P18" s="4">
         <v>2023</v>
@@ -51098,7 +51102,7 @@
         <v>2023</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>11</v>
@@ -51119,10 +51123,10 @@
         <v>2952</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>32</v>
@@ -51131,7 +51135,7 @@
         <v>32</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="P19" s="4">
         <v>2023</v>
@@ -51151,7 +51155,7 @@
         <v>2023</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>11</v>
@@ -51172,10 +51176,10 @@
         <v>43</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>32</v>
@@ -51184,7 +51188,7 @@
         <v>32</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="P20" s="4">
         <v>2023</v>
@@ -51204,7 +51208,7 @@
         <v>2023</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>11</v>
@@ -51225,10 +51229,10 @@
         <v>0</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>32</v>
@@ -51237,7 +51241,7 @@
         <v>32</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="P21" s="4">
         <v>2023</v>
@@ -51257,7 +51261,7 @@
         <v>2023</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>11</v>
@@ -51278,19 +51282,19 @@
         <v>4154</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="P22" s="4">
         <v>2023</v>
@@ -51310,7 +51314,7 @@
         <v>2023</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>11</v>
@@ -51331,19 +51335,19 @@
         <v>3000</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="P23" s="4">
         <v>2023</v>
@@ -51363,7 +51367,7 @@
         <v>2023</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>11</v>
@@ -51384,19 +51388,19 @@
         <v>162</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="P24" s="4">
         <v>2023</v>
@@ -51416,7 +51420,7 @@
         <v>2023</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>11</v>
@@ -51437,19 +51441,19 @@
         <v>0</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P25" s="4">
         <v>2023</v>
@@ -51469,7 +51473,7 @@
         <v>2023</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>11</v>
@@ -51481,7 +51485,7 @@
         <v>51</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>14</v>
@@ -51490,19 +51494,19 @@
         <v>14247</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P26" s="4">
         <v>2023</v>
@@ -51522,7 +51526,7 @@
         <v>2023</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>11</v>
@@ -51534,7 +51538,7 @@
         <v>51</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>14</v>
@@ -51543,19 +51547,19 @@
         <v>14250</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P27" s="4">
         <v>2023</v>
@@ -51575,7 +51579,7 @@
         <v>2023</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>12</v>
@@ -51596,19 +51600,19 @@
         <v>0</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P28" s="4">
         <v>2023</v>
@@ -51628,7 +51632,7 @@
         <v>2023</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>12</v>
@@ -51649,19 +51653,19 @@
         <v>0</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P29" s="4">
         <v>2023</v>
@@ -51681,7 +51685,7 @@
         <v>2023</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>12</v>
@@ -51702,19 +51706,19 @@
         <v>0</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P30" s="4">
         <v>2023</v>
@@ -51734,7 +51738,7 @@
         <v>2023</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>12</v>
@@ -51755,19 +51759,19 @@
         <v>0</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P31" s="4">
         <v>2023</v>
@@ -51787,7 +51791,7 @@
         <v>2023</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>12</v>
@@ -51808,19 +51812,19 @@
         <v>0</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P32" s="4">
         <v>2023</v>
@@ -51840,13 +51844,13 @@
         <v>2023</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>51</v>
@@ -51855,10 +51859,10 @@
         <v>19</v>
       </c>
       <c r="J33" s="7">
-        <v>0.54877848827676701</v>
+        <v>0.5520696388379619</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>25</v>
@@ -51890,13 +51894,13 @@
         <v>2023</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>51</v>
@@ -51908,7 +51912,7 @@
         <v>0.43613707165109</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>25</v>
@@ -51940,13 +51944,13 @@
         <v>2023</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>51</v>
@@ -51955,10 +51959,10 @@
         <v>23</v>
       </c>
       <c r="J35" s="7">
-        <v>1.5084440072142999E-2</v>
+        <v>1.1793289510948164E-2</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
updated initial mapping file
</commit_message>
<xml_diff>
--- a/termNIT/2023/TERMNIT_mapping_2023.xlsx
+++ b/termNIT/2023/TERMNIT_mapping_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\WCVI_Chinook_Term_Run_Recon\WCVI_CN_TermRunRecon\termNIT\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832F2970-95A8-45A5-AEBC-78F4EDB8DA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E54C84-8DB0-417B-A0B7-6CAB6F70DB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{E2731BFC-E1F4-4F7A-AD91-46B95AB44FF5}"/>
   </bookViews>
@@ -230,7 +230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="92">
   <si>
     <t>FSC</t>
   </si>
@@ -302,9 +302,6 @@
   </si>
   <si>
     <t>Jack</t>
-  </si>
-  <si>
-    <t>Broostock corrected</t>
   </si>
   <si>
     <t>NA</t>
@@ -416,9 +413,6 @@
   </si>
   <si>
     <t>What temporal strata (or substrata) should be used for pooling (or not pooling) stock comp data?</t>
-  </si>
-  <si>
-    <t>Broostock corrected - Total</t>
   </si>
   <si>
     <t>Broodstock corrected - Total</t>
@@ -947,66 +941,66 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1014,39 +1008,39 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -50176,7 +50170,7 @@
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50205,89 +50199,89 @@
   <sheetData>
     <row r="1" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="S2" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2023</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>19</v>
@@ -50296,48 +50290,48 @@
         <v>22</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P3" s="4">
         <v>2023</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S3" s="4">
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2023</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>20</v>
@@ -50346,48 +50340,48 @@
         <v>22</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P4" s="4">
         <v>2023</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S4" s="4">
         <v>2022</v>
       </c>
     </row>
-    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2023</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>15</v>
@@ -50399,42 +50393,42 @@
         <v>900</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P5" s="4">
         <v>2023</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S5" s="4">
         <v>2022</v>
       </c>
     </row>
-    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2023</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>1</v>
@@ -50452,42 +50446,42 @@
         <v>4768</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P6" s="4">
         <v>2023</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S6" s="4">
         <v>2022</v>
       </c>
     </row>
-    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>2023</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>1</v>
@@ -50505,42 +50499,42 @@
         <v>3233</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P7" s="4">
         <v>2023</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S7" s="4">
         <v>2022</v>
       </c>
     </row>
-    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2023</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>1</v>
@@ -50558,39 +50552,39 @@
         <v>8001</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P8" s="4">
         <v>2023</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S8" s="4">
         <v>2022</v>
       </c>
     </row>
-    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2023</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>2</v>
@@ -50605,25 +50599,25 @@
         <v>21</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J9" s="4">
         <v>277</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P9" s="4">
         <v>2023</v>
@@ -50632,18 +50626,18 @@
         <v>21</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S9" s="4">
         <v>2022</v>
       </c>
     </row>
-    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2023</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>2</v>
@@ -50658,45 +50652,45 @@
         <v>21</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J10" s="4">
         <v>6</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P10" s="4">
         <v>2023</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S10" s="4">
         <v>2022</v>
       </c>
     </row>
-    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>2023</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>2</v>
@@ -50711,45 +50705,45 @@
         <v>21</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J11" s="4">
         <v>0</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2023</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>2</v>
@@ -50767,39 +50761,39 @@
         <v>0</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2023</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>2</v>
@@ -50817,39 +50811,39 @@
         <v>0</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>2023</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>2</v>
@@ -50867,39 +50861,39 @@
         <v>0</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P14" s="4">
         <v>2023</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S14" s="4">
         <v>2022</v>
       </c>
     </row>
-    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2023</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>2</v>
@@ -50917,39 +50911,39 @@
         <v>300</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P15" s="4">
         <v>2023</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S15" s="4">
         <v>2022</v>
       </c>
     </row>
-    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>2023</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>6</v>
@@ -50958,7 +50952,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16" s="3">
         <v>22</v>
@@ -50967,39 +50961,39 @@
         <v>0</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>2023</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>6</v>
@@ -51008,7 +51002,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="3">
         <v>22</v>
@@ -51017,31 +51011,31 @@
         <v>0</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -51049,49 +51043,49 @@
         <v>2023</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J18" s="4">
         <v>2747</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P18" s="4">
         <v>2023</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S18" s="4">
         <v>2022</v>
@@ -51102,49 +51096,49 @@
         <v>2023</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J19" s="4">
         <v>2952</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="P19" s="4">
         <v>2023</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S19" s="4">
         <v>2022</v>
@@ -51155,49 +51149,49 @@
         <v>2023</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J20" s="4">
         <v>43</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P20" s="4">
         <v>2023</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S20" s="4">
         <v>2022</v>
@@ -51208,49 +51202,49 @@
         <v>2023</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J21" s="4">
         <v>0</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P21" s="4">
         <v>2023</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S21" s="4">
         <v>2022</v>
@@ -51261,7 +51255,7 @@
         <v>2023</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>11</v>
@@ -51270,40 +51264,40 @@
         <v>9</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J22" s="4">
         <v>4154</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P22" s="4">
         <v>2023</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S22" s="4">
         <v>2022</v>
@@ -51314,7 +51308,7 @@
         <v>2023</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>11</v>
@@ -51323,40 +51317,40 @@
         <v>9</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J23" s="4">
         <v>3000</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P23" s="4">
         <v>2023</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S23" s="4">
         <v>2022</v>
@@ -51367,7 +51361,7 @@
         <v>2023</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>11</v>
@@ -51376,40 +51370,40 @@
         <v>9</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J24" s="4">
         <v>162</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P24" s="4">
         <v>2023</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S24" s="4">
         <v>2022</v>
@@ -51420,7 +51414,7 @@
         <v>2023</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>11</v>
@@ -51429,40 +51423,40 @@
         <v>9</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J25" s="4">
         <v>0</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P25" s="4">
         <v>2023</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S25" s="4">
         <v>2022</v>
@@ -51473,7 +51467,7 @@
         <v>2023</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>11</v>
@@ -51482,10 +51476,10 @@
         <v>10</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>14</v>
@@ -51494,28 +51488,28 @@
         <v>14247</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P26" s="4">
         <v>2023</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S26" s="4">
         <v>2022</v>
@@ -51526,7 +51520,7 @@
         <v>2023</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>11</v>
@@ -51535,10 +51529,10 @@
         <v>10</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>14</v>
@@ -51547,28 +51541,28 @@
         <v>14250</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P27" s="4">
         <v>2023</v>
       </c>
       <c r="Q27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S27" s="4">
         <v>2022</v>
@@ -51579,7 +51573,7 @@
         <v>2023</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>12</v>
@@ -51588,7 +51582,7 @@
         <v>10</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>15</v>
@@ -51600,28 +51594,28 @@
         <v>0</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P28" s="4">
         <v>2023</v>
       </c>
       <c r="Q28" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S28" s="4">
         <v>2022</v>
@@ -51632,7 +51626,7 @@
         <v>2023</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>12</v>
@@ -51641,40 +51635,40 @@
         <v>10</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J29" s="4">
         <v>0</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P29" s="4">
         <v>2023</v>
       </c>
       <c r="Q29" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S29" s="4">
         <v>2022</v>
@@ -51685,7 +51679,7 @@
         <v>2023</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>12</v>
@@ -51694,40 +51688,40 @@
         <v>10</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J30" s="4">
         <v>0</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P30" s="4">
         <v>2023</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S30" s="4">
         <v>2022</v>
@@ -51738,7 +51732,7 @@
         <v>2023</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>12</v>
@@ -51747,40 +51741,40 @@
         <v>10</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J31" s="4">
         <v>0</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P31" s="4">
         <v>2023</v>
       </c>
       <c r="Q31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S31" s="4">
         <v>2022</v>
@@ -51791,7 +51785,7 @@
         <v>2023</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>12</v>
@@ -51800,40 +51794,40 @@
         <v>10</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J32" s="4">
         <v>0</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P32" s="4">
         <v>2023</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R32" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S32" s="4">
         <v>2022</v>
@@ -51844,16 +51838,16 @@
         <v>2023</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>19</v>
@@ -51862,31 +51856,31 @@
         <v>0.5520696388379619</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P33" s="4">
         <v>2023</v>
       </c>
       <c r="Q33" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R33" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S33" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -51894,16 +51888,16 @@
         <v>2023</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>20</v>
@@ -51912,31 +51906,31 @@
         <v>0.43613707165109</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O34" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P34" s="4">
         <v>2023</v>
       </c>
       <c r="Q34" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R34" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S34" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -51944,16 +51938,16 @@
         <v>2023</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>23</v>
@@ -51962,31 +51956,31 @@
         <v>1.1793289510948164E-2</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O35" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P35" s="4">
         <v>2023</v>
       </c>
       <c r="Q35" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S35" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated NITmap to account for new additions of rec catch and sampling data
</commit_message>
<xml_diff>
--- a/termNIT/2023/TERMNIT_mapping_2023.xlsx
+++ b/termNIT/2023/TERMNIT_mapping_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\WCVI_Chinook_Term_Run_Recon\WCVI_CN_TermRunRecon\termNIT\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50A7C70-834F-4C32-BA86-BCC0E962E57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7C4824-828F-4AB1-A28F-9581BFE85AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{E2731BFC-E1F4-4F7A-AD91-46B95AB44FF5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="termNIT_map" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">termNIT_map!$C$2:$R$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">termNIT_map!$C$2:$R$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -103,7 +103,177 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{5B52FA44-BC21-4958-982C-073547684942}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{73920EF5-609F-4F09-8704-67DE95DECC6D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Katie Davidson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Manual data entry in this column (for now)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{213CC5A4-0C3F-44B3-8959-C18EB433661D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Katie Davidson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+note that june isn't usually included for catch estimate (enumeration), but we will sometimes retain june biodata to pool into July if sample sizes are low.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{1FC0E9A6-483E-48C0-B12E-BC206AD1C6DD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Katie Davidson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+note that june isn't usually included for catch estimate (enumeration), but we will sometimes retain june biodata to pool into July if sample sizes are low.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M9" authorId="0" shapeId="0" xr:uid="{A1693708-B9F6-46B7-B3A5-BAF2B3F1B4E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Katie Davidson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+note that june isn't usually included for catch estimate (enumeration), but we will sometimes retain june biodata to pool into July if sample sizes are low.
+Usually pooled over sub-areas and months due to low sample size.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{1EA1C871-70C6-4BD2-BE1F-53A56A4FC49B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Katie Davidson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+note that june isn't usually included for catch estimate (enumeration), but we will sometimes retain june biodata to pool into July if sample sizes are low.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{93BDB0E0-E60B-488B-9C23-1E16E308C0FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Katie Davidson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+note that june isn't usually included for catch estimate (enumeration), but we will sometimes retain june biodata to pool into July if sample sizes are low.
+Usually pooled over sub-areas and months due to low sample size.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q10" authorId="0" shapeId="0" xr:uid="{B46541BF-3F1E-4C64-9B7E-F44D31748C9B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Katie Davidson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+note that june isn't usually included for catch estimate (enumeration), but we will sometimes retain june biodata to pool into July if sample sizes are low.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{5B52FA44-BC21-4958-982C-073547684942}">
       <text>
         <r>
           <rPr>
@@ -127,7 +297,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{FB339F80-1603-4252-BC3F-E11C1970832E}">
+    <comment ref="M11" authorId="0" shapeId="0" xr:uid="{BEEA84EC-F031-4AE0-B641-65DDF8D4514A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Katie Davidson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+note that june isn't usually included for catch estimate (enumeration), but we will sometimes retain june biodata to pool into July if sample sizes are low.
+Usually pooled over sub-areas and months due to low sample size.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{FB339F80-1603-4252-BC3F-E11C1970832E}">
       <text>
         <r>
           <rPr>
@@ -151,7 +346,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{0FC994F5-0623-42B9-A37D-3BDEA986D05C}">
+    <comment ref="M12" authorId="0" shapeId="0" xr:uid="{4DDBEAA3-07C8-4231-B52D-CCD79EC398F2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Katie Davidson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+note that june isn't usually included for catch estimate (enumeration), but we will sometimes retain june biodata to pool into July if sample sizes are low.
+Usually pooled over sub-areas and months due to low sample size.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{0FC994F5-0623-42B9-A37D-3BDEA986D05C}">
       <text>
         <r>
           <rPr>
@@ -175,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{61787744-B0CB-4EE1-A870-0418371F02D9}">
+    <comment ref="E17" authorId="0" shapeId="0" xr:uid="{61787744-B0CB-4EE1-A870-0418371F02D9}">
       <text>
         <r>
           <rPr>
@@ -200,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="0" shapeId="0" xr:uid="{8278C857-0BE4-4149-91EA-A8C955DB917A}">
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{8278C857-0BE4-4149-91EA-A8C955DB917A}">
       <text>
         <r>
           <rPr>
@@ -230,7 +450,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="94">
   <si>
     <t>FSC</t>
   </si>
@@ -507,12 +727,18 @@
   <si>
     <t>Broodstock corrected - Males (incl Jacks)</t>
   </si>
+  <si>
+    <t>UNLESS GRAY, IN WHICH CASE AUTO-POPULATES FROM R CODE</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,8 +782,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -576,6 +815,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -590,7 +835,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -613,6 +858,10 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9798D8-54AF-4090-A250-C882BB064B7E}">
-  <dimension ref="A3:B16387"/>
+  <dimension ref="A3:Q16387"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,7 +1188,7 @@
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -947,7 +1196,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
@@ -955,7 +1204,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -963,7 +1212,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -971,7 +1220,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -979,7 +1228,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -987,7 +1236,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
@@ -995,7 +1244,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -1003,47 +1252,87 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L12" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L13" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L14" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="L15" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -50167,10 +50456,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD15511-D0E0-440B-B215-63E04B9AC67B}">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50593,7 +50882,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="H9" s="3">
         <v>21</v>
@@ -50601,36 +50890,19 @@
       <c r="I9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="4">
-        <v>277</v>
-      </c>
+      <c r="J9" s="8"/>
       <c r="K9" s="4" t="s">
         <v>69</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
       <c r="O9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P9" s="4">
-        <v>2023</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="R9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="S9" s="4">
-        <v>2022</v>
-      </c>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -50646,7 +50918,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" s="3">
         <v>21</v>
@@ -50654,29 +50926,21 @@
       <c r="I10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J10" s="4">
-        <v>6</v>
-      </c>
+      <c r="J10" s="8"/>
       <c r="K10" s="4" t="s">
         <v>69</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
       <c r="O10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P10" s="4">
-        <v>2023</v>
-      </c>
+      <c r="P10" s="8"/>
       <c r="Q10" s="4" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>29</v>
@@ -50699,7 +50963,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H11" s="3">
         <v>21</v>
@@ -50707,35 +50971,27 @@
       <c r="I11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="4">
-        <v>0</v>
-      </c>
+      <c r="J11" s="8"/>
       <c r="K11" s="4" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
       <c r="O11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P11" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="P11" s="8"/>
       <c r="Q11" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="S11" s="4">
+        <v>2022</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -50749,35 +51005,30 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H12" s="3">
-        <v>22</v>
-      </c>
-      <c r="J12" s="4">
-        <v>0</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="8"/>
       <c r="K12" s="4" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
       <c r="O12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P12" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="P12" s="8"/>
       <c r="Q12" s="4" t="s">
         <v>24</v>
       </c>
@@ -50802,7 +51053,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H13" s="3">
         <v>22</v>
@@ -50849,10 +51100,10 @@
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H14" s="3">
         <v>22</v>
@@ -50861,31 +51112,31 @@
         <v>0</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="P14" s="4">
-        <v>2023</v>
+        <v>24</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="S14" s="4">
-        <v>2022</v>
+        <v>24</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -50902,13 +51153,13 @@
         <v>5</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H15" s="3">
         <v>22</v>
       </c>
       <c r="J15" s="4">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>68</v>
@@ -50946,46 +51197,46 @@
         <v>73</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H16" s="3">
         <v>22</v>
       </c>
       <c r="J16" s="4">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>24</v>
+        <v>61</v>
+      </c>
+      <c r="P16" s="4">
+        <v>2023</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S16" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="S16" s="4">
+        <v>2022</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -50999,7 +51250,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>24</v>
@@ -51043,52 +51294,49 @@
         <v>2023</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>48</v>
+        <v>24</v>
+      </c>
+      <c r="H18" s="3">
+        <v>22</v>
       </c>
       <c r="J18" s="4">
-        <v>2747</v>
+        <v>0</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="P18" s="4">
-        <v>2023</v>
+        <v>24</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="S18" s="4">
-        <v>2022</v>
+        <v>24</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -51108,13 +51356,13 @@
         <v>50</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>48</v>
       </c>
       <c r="J19" s="4">
-        <v>2952</v>
+        <v>2747</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>69</v>
@@ -51129,7 +51377,7 @@
         <v>31</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P19" s="4">
         <v>2023</v>
@@ -51161,13 +51409,13 @@
         <v>50</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>48</v>
       </c>
       <c r="J20" s="4">
-        <v>43</v>
+        <v>2952</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>69</v>
@@ -51182,7 +51430,7 @@
         <v>31</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P20" s="4">
         <v>2023</v>
@@ -51214,13 +51462,13 @@
         <v>50</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>48</v>
       </c>
       <c r="J21" s="4">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>69</v>
@@ -51235,7 +51483,7 @@
         <v>31</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="P21" s="4">
         <v>2023</v>
@@ -51261,34 +51509,34 @@
         <v>11</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>50</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>48</v>
       </c>
       <c r="J22" s="4">
-        <v>4154</v>
+        <v>0</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="P22" s="4">
         <v>2023</v>
@@ -51320,13 +51568,13 @@
         <v>50</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>48</v>
       </c>
       <c r="J23" s="4">
-        <v>3000</v>
+        <v>4154</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>68</v>
@@ -51341,7 +51589,7 @@
         <v>90</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="P23" s="4">
         <v>2023</v>
@@ -51373,13 +51621,13 @@
         <v>50</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>48</v>
       </c>
       <c r="J24" s="4">
-        <v>162</v>
+        <v>3000</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>68</v>
@@ -51394,7 +51642,7 @@
         <v>90</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="P24" s="4">
         <v>2023</v>
@@ -51426,13 +51674,13 @@
         <v>50</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>48</v>
       </c>
       <c r="J25" s="4">
-        <v>0</v>
+        <v>162</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>68</v>
@@ -51447,7 +51695,7 @@
         <v>90</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="P25" s="4">
         <v>2023</v>
@@ -51473,19 +51721,19 @@
         <v>11</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>50</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="J26" s="4">
-        <v>14247</v>
+        <v>0</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>68</v>
@@ -51532,13 +51780,13 @@
         <v>50</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J27" s="4">
-        <v>14250</v>
+        <v>14247</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>68</v>
@@ -51576,7 +51824,7 @@
         <v>72</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>10</v>
@@ -51585,13 +51833,13 @@
         <v>50</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J28" s="4">
-        <v>0</v>
+        <v>14250</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>68</v>
@@ -51641,7 +51889,7 @@
         <v>15</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="J29" s="4">
         <v>0</v>
@@ -51694,7 +51942,7 @@
         <v>15</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J30" s="4">
         <v>0</v>
@@ -51747,7 +51995,7 @@
         <v>15</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J31" s="4">
         <v>0</v>
@@ -51800,7 +52048,7 @@
         <v>15</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J32" s="4">
         <v>0</v>
@@ -51841,46 +52089,49 @@
         <v>72</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>50</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J33" s="7">
-        <v>0.5520696388379619</v>
+        <v>15</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J33" s="4">
+        <v>0</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="P33" s="4">
         <v>2023</v>
       </c>
       <c r="Q33" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="R33" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S33" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="S33" s="4">
+        <v>2022</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -51900,10 +52151,10 @@
         <v>50</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J34" s="7">
-        <v>0.43613707165109</v>
+        <v>0.5520696388379619</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>69</v>
@@ -51950,10 +52201,10 @@
         <v>50</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J35" s="7">
-        <v>1.1793289510948164E-2</v>
+        <v>0.43613707165109</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>69</v>
@@ -51980,6 +52231,56 @@
         <v>24</v>
       </c>
       <c r="S35" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" s="7">
+        <v>1.1793289510948164E-2</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P36" s="4">
+        <v>2023</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S36" s="4" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>